<commit_message>
Commit Master GS Partial Fix(edit not yet and lead time in create and edit not yet), Master Vehicle Spect Upload fix(add upload image)
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/masterVehicleSpect.xlsx
+++ b/FMS.Website/files_upload/masterVehicleSpect.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Master Vehicle Spect</t>
   </si>
@@ -82,21 +82,34 @@
     <t>Gasoline</t>
   </si>
   <si>
-    <t>GLS 2.0 A/T</t>
-  </si>
-  <si>
     <t>Automatic</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>C:\Users\pc\Pictures\FMS\FlowChart\CAF_Page_Edited.png</t>
+  </si>
+  <si>
+    <t>PX 2.0 A/T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -162,13 +175,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -467,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -484,28 +499,30 @@
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" ht="23.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -537,35 +554,38 @@
         <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -583,17 +603,20 @@
       <c r="J3" s="2">
         <v>0</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="2"/>
+      <c r="P3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>